<commit_message>
flappy bird part I
</commit_message>
<xml_diff>
--- a/Tanmenet.xlsx
+++ b/Tanmenet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
   <si>
     <t xml:space="preserve">Sorszám</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t xml:space="preserve">HTML+JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flappy bird clouds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hangosítás 17:00-től</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tantestületi ebéd 14:00-től</t>
   </si>
   <si>
     <t xml:space="preserve">NINCS</t>
@@ -67,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,24 +143,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,421 +314,430 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <f aca="false">B3-7</f>
         <v>45960</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="2" t="n">
         <f aca="false">A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <f aca="false">B4-7</f>
         <v>45967</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="2" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <f aca="false">DATE(2025,11,13)</f>
         <v>45974</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="2" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <f aca="false">B4+7</f>
         <v>45981</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="2" t="n">
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <f aca="false">B5+7</f>
         <v>45988</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="2" t="n">
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <f aca="false">B6+7</f>
         <v>45995</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="2" t="n">
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <f aca="false">B7+7</f>
         <v>46002</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="2" t="n">
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <f aca="false">B8+7</f>
         <v>46009</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>5</v>
+      <c r="D9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="2" t="n">
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <f aca="false">B9+7</f>
         <v>46016</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3"/>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="2" t="n">
         <f aca="false">A10+1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
         <f aca="false">B10+7</f>
         <v>46023</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3"/>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="2" t="n">
         <f aca="false">A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <f aca="false">B11+7</f>
         <v>46030</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="2" t="n">
         <f aca="false">A12+1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="3" t="n">
         <f aca="false">B12+7</f>
         <v>46037</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="2" t="n">
         <f aca="false">A13+1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <f aca="false">B13+7</f>
         <v>46044</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="2" t="n">
         <f aca="false">A14+1</f>
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="3" t="n">
         <f aca="false">B14+7</f>
         <v>46051</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="2" t="n">
         <f aca="false">A15+1</f>
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="3" t="n">
         <f aca="false">B15+7</f>
         <v>46058</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="2" t="n">
         <f aca="false">A16+1</f>
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="3" t="n">
         <f aca="false">B16+7</f>
         <v>46065</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="2" t="n">
         <f aca="false">A17+1</f>
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="3" t="n">
         <f aca="false">B17+7</f>
         <v>46072</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="2" t="n">
         <f aca="false">A18+1</f>
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="3" t="n">
         <f aca="false">B18+7</f>
         <v>46079</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="2" t="n">
         <f aca="false">A19+1</f>
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="3" t="n">
         <f aca="false">B19+7</f>
         <v>46086</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="2" t="n">
         <f aca="false">A20+1</f>
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="3" t="n">
         <f aca="false">B20+7</f>
         <v>46093</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="2" t="n">
         <f aca="false">A21+1</f>
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="3" t="n">
         <f aca="false">B21+7</f>
         <v>46100</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="2" t="n">
         <f aca="false">A22+1</f>
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="3" t="n">
         <f aca="false">B22+7</f>
         <v>46107</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="2" t="n">
         <f aca="false">A23+1</f>
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <f aca="false">B23+7</f>
         <v>46114</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3"/>
+      <c r="C24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="2" t="n">
         <f aca="false">A24+1</f>
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="3" t="n">
         <f aca="false">B24+7</f>
         <v>46121</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3"/>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="2" t="n">
         <f aca="false">A25+1</f>
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="3" t="n">
         <f aca="false">B25+7</f>
         <v>46128</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="2" t="n">
         <f aca="false">A26+1</f>
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="3" t="n">
         <f aca="false">B26+7</f>
         <v>46135</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="2" t="n">
         <f aca="false">A27+1</f>
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="3" t="n">
         <f aca="false">B27+7</f>
         <v>46142</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="2" t="n">
         <f aca="false">A28+1</f>
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="3" t="n">
         <f aca="false">B28+7</f>
         <v>46149</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="2" t="n">
         <f aca="false">A29+1</f>
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="3" t="n">
         <f aca="false">B29+7</f>
         <v>46156</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="2" t="n">
         <f aca="false">A30+1</f>
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="3" t="n">
         <f aca="false">B30+7</f>
         <v>46163</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="3"/>
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="2" t="n">
         <f aca="false">A31+1</f>
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="3" t="n">
         <f aca="false">B31+7</f>
         <v>46170</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="3" t="n">
+      <c r="D33" s="4" t="n">
         <f aca="false">COUNTIF(D2:D32,D2)</f>
         <v>25</v>
       </c>
@@ -723,8 +747,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -736,13 +760,13 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -760,141 +784,141 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <f aca="false">DATE(2025,9,11)</f>
         <v>45911</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="3" t="n">
         <f aca="false">B2+7</f>
         <v>45918</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <f aca="false">B3+7</f>
         <v>45925</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <f aca="false">B4+7</f>
         <v>45932</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="n">
+      <c r="A6" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <f aca="false">B5+7</f>
         <v>45939</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="3" t="n">
         <f aca="false">B6+7</f>
         <v>45946</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2"/>
+      <c r="B22" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add initial documentation for container concepts and usage
</commit_message>
<xml_diff>
--- a/Tanmenet.xlsx
+++ b/Tanmenet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t xml:space="preserve">Sorszám</t>
   </si>
@@ -50,7 +50,16 @@
     <t xml:space="preserve">Flappy bird clouds</t>
   </si>
   <si>
+    <t xml:space="preserve">Flappy bird player</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hangosítás 17:00-től</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELMARADT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adatbázis.ppt</t>
   </si>
   <si>
     <t xml:space="preserve">Tantestületi ebéd 14:00-től</t>
@@ -294,7 +303,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -369,7 +378,7 @@
         <f aca="false">B4+7</f>
         <v>45981</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -385,11 +394,14 @@
         <f aca="false">B5+7</f>
         <v>45988</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>9</v>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,9 +413,10 @@
         <f aca="false">B6+7</f>
         <v>45995</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -414,6 +427,9 @@
         <f aca="false">B7+7</f>
         <v>46002</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
@@ -427,11 +443,12 @@
         <f aca="false">B8+7</f>
         <v>46009</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>10</v>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +461,7 @@
         <v>46016</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4"/>
     </row>
@@ -458,7 +475,7 @@
         <v>46023</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4"/>
     </row>
@@ -628,7 +645,7 @@
         <v>46114</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -642,7 +659,7 @@
         <v>46121</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D25" s="4"/>
     </row>
@@ -721,7 +738,7 @@
         <v>46163</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D31" s="4"/>
     </row>
@@ -739,7 +756,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="4" t="n">
         <f aca="false">COUNTIF(D2:D32,D2)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +764,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -917,8 +934,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Általános"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Általános"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>